<commit_message>
Updated the table format and structure
</commit_message>
<xml_diff>
--- a/Validation_and_Testing_results.xlsx
+++ b/Validation_and_Testing_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofc-my.sharepoint.com/personal/sujesh_padhi1_ucalgary_ca/Documents/02_Winter23/02_CPSC_601.27/03_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{819622FB-5E62-48E8-864D-29A98BFB803B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F66EA4D0-55B2-44BA-8BCF-1B7E41A23F42}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{819622FB-5E62-48E8-864D-29A98BFB803B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61B476BA-E674-459D-A2F7-323F7754AFFA}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="1065" windowWidth="22095" windowHeight="10875" activeTab="1" xr2:uid="{B17FBFDA-8A5E-47C7-8928-68C91A352C89}"/>
+    <workbookView xWindow="3450" yWindow="1065" windowWidth="22095" windowHeight="11775" activeTab="1" xr2:uid="{B17FBFDA-8A5E-47C7-8928-68C91A352C89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="19">
   <si>
     <t>TO</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Language Mapping</t>
+  </si>
+  <si>
+    <t>English mappings</t>
+  </si>
+  <si>
+    <t>Non-English mappings</t>
   </si>
 </sst>
 </file>
@@ -95,7 +101,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -155,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -298,9 +304,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -311,14 +315,154 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -327,8 +471,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -338,30 +515,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -371,28 +524,49 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -410,6 +584,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -715,164 +893,164 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="10"/>
-    <col min="11" max="11" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="10"/>
-    <col min="16" max="16" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="7"/>
+    <col min="11" max="11" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="7"/>
+    <col min="16" max="16" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="8"/>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="7"/>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -885,387 +1063,405 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997B4389-6C04-4425-8F8F-6838C51EBC3B}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="10" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="3" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="17" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="17" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="D3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G3" s="24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="19">
+      <c r="D5" s="10">
         <v>0.19600000000000001</v>
       </c>
-      <c r="D3" s="19">
+      <c r="E5" s="10">
         <v>0.438</v>
       </c>
-      <c r="E3" s="19">
+      <c r="F5" s="10">
         <v>0.19500000000000001</v>
       </c>
-      <c r="F3" s="19">
+      <c r="G5" s="28">
         <v>0.42</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19">
+      <c r="D6" s="10">
         <v>0.247</v>
       </c>
-      <c r="D4" s="19">
+      <c r="E6" s="10">
         <v>0.73699999999999999</v>
       </c>
-      <c r="E4" s="19">
+      <c r="F6" s="10">
         <v>0.25</v>
       </c>
-      <c r="F4" s="19">
+      <c r="G6" s="28">
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="C7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="19">
+      <c r="D7" s="10">
         <v>0.183</v>
       </c>
-      <c r="D5" s="19">
+      <c r="E7" s="10">
         <v>0.67</v>
       </c>
-      <c r="E5" s="19">
+      <c r="F7" s="10">
         <v>0.187</v>
       </c>
-      <c r="F5" s="19">
+      <c r="G7" s="28">
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="C8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="19">
+      <c r="D8" s="10">
         <v>0.26300000000000001</v>
       </c>
-      <c r="D6" s="19">
+      <c r="E8" s="10">
         <v>0.64400000000000002</v>
       </c>
-      <c r="E6" s="19">
+      <c r="F8" s="10">
         <v>0.254</v>
       </c>
-      <c r="F6" s="19">
+      <c r="G8" s="28">
         <v>0.68</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="C9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="19">
+      <c r="D9" s="10">
         <v>0.152</v>
       </c>
-      <c r="D7" s="19">
+      <c r="E9" s="10">
         <v>0.53800000000000003</v>
       </c>
-      <c r="E7" s="19">
+      <c r="F9" s="10">
         <v>0.21</v>
       </c>
-      <c r="F7" s="19">
+      <c r="G9" s="28">
         <v>0.41499999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="C10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="19">
+      <c r="D10" s="10">
         <v>0.20200000000000001</v>
       </c>
-      <c r="D8" s="19">
+      <c r="E10" s="10">
         <v>0.90900000000000003</v>
       </c>
-      <c r="E8" s="19">
+      <c r="F10" s="10">
         <v>0.27300000000000002</v>
       </c>
-      <c r="F8" s="19">
+      <c r="G10" s="28">
         <v>0.68300000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="C11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="19">
+      <c r="D11" s="10">
         <v>0.17100000000000001</v>
       </c>
-      <c r="D9" s="19">
+      <c r="E11" s="10">
         <v>0.61299999999999999</v>
       </c>
-      <c r="E9" s="19">
+      <c r="F11" s="10">
         <v>0.192</v>
       </c>
-      <c r="F9" s="19">
+      <c r="G11" s="28">
         <v>0.58899999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="C12" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="19">
+      <c r="D12" s="10">
         <v>0.27900000000000003</v>
       </c>
-      <c r="D10" s="19">
+      <c r="E12" s="10">
         <v>0.63200000000000001</v>
       </c>
-      <c r="E10" s="19">
+      <c r="F12" s="10">
         <v>0.27700000000000002</v>
       </c>
-      <c r="F10" s="19">
+      <c r="G12" s="28">
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="C13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="19">
+      <c r="D13" s="10">
         <v>0.21</v>
       </c>
-      <c r="D11" s="19">
+      <c r="E13" s="10">
         <v>0.57399999999999995</v>
       </c>
-      <c r="E11" s="19">
+      <c r="F13" s="10">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F11" s="19">
+      <c r="G13" s="28">
         <v>0.47199999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="C14" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="19">
+      <c r="D14" s="10">
         <v>0.23</v>
       </c>
-      <c r="D12" s="19">
+      <c r="E14" s="10">
         <v>0.76400000000000001</v>
       </c>
-      <c r="E12" s="19">
+      <c r="F14" s="10">
         <v>0.30499999999999999</v>
       </c>
-      <c r="F12" s="19">
+      <c r="G14" s="28">
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="C16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="19">
+      <c r="D16" s="10">
         <v>0.10299999999999999</v>
       </c>
-      <c r="D14" s="19">
+      <c r="E16" s="10">
         <v>0.61899999999999999</v>
       </c>
-      <c r="E14" s="19">
+      <c r="F16" s="10">
         <v>0.13</v>
       </c>
-      <c r="F14" s="19">
+      <c r="G16" s="28">
         <v>0.51500000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="C17" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="19">
+      <c r="D17" s="10">
         <v>0.108</v>
       </c>
-      <c r="D15" s="19">
+      <c r="E17" s="10">
         <v>0.64200000000000002</v>
       </c>
-      <c r="E15" s="19">
+      <c r="F17" s="10">
         <v>0.126</v>
       </c>
-      <c r="F15" s="19">
+      <c r="G17" s="28">
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="C18" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="19">
+      <c r="D18" s="10">
         <v>0.115</v>
       </c>
-      <c r="D16" s="19">
+      <c r="E18" s="10">
         <v>0.57399999999999995</v>
       </c>
-      <c r="E16" s="19">
+      <c r="F18" s="10">
         <v>0.13700000000000001</v>
       </c>
-      <c r="F16" s="19">
+      <c r="G18" s="28">
         <v>0.50700000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="C19" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="19">
+      <c r="D19" s="10">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="D17" s="19">
+      <c r="E19" s="10">
         <v>0.89400000000000002</v>
       </c>
-      <c r="E17" s="19">
+      <c r="F19" s="10">
         <v>0.121</v>
       </c>
-      <c r="F17" s="19">
+      <c r="G19" s="28">
         <v>0.746</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="C20" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="19">
+      <c r="D20" s="10">
         <v>0.14599999999999999</v>
       </c>
-      <c r="D18" s="19">
+      <c r="E20" s="10">
         <v>0.499</v>
       </c>
-      <c r="E18" s="19">
+      <c r="F20" s="10">
         <v>0.154</v>
       </c>
-      <c r="F18" s="19">
+      <c r="G20" s="28">
         <v>0.51300000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="C21" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="19">
+      <c r="D21" s="31">
         <v>0.115</v>
       </c>
-      <c r="D19" s="19">
+      <c r="E21" s="31">
         <v>0.78800000000000003</v>
       </c>
-      <c r="E19" s="19">
+      <c r="F21" s="31">
         <v>0.13200000000000001</v>
       </c>
-      <c r="F19" s="19">
+      <c r="G21" s="32">
         <v>0.73199999999999998</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A1:B1"/>
+  <mergeCells count="5">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>